<commit_message>
Update extraction notebook and refreshed all_schools.xlsx
</commit_message>
<xml_diff>
--- a/output_Balance_Sheet_DS/all_schools.xlsx
+++ b/output_Balance_Sheet_DS/all_schools.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH20"/>
+  <dimension ref="A1:AJ20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -599,6 +599,16 @@
           <t>noncontrolling_interest</t>
         </is>
       </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>other_assets_plug</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>other_liabilities_plug</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -693,6 +703,12 @@
         <v>2297576</v>
       </c>
       <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="n">
+        <v>-480373</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>-588106</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -791,6 +807,12 @@
         <v>528400</v>
       </c>
       <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="n">
+        <v>3390</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>-10468</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -891,6 +913,12 @@
         <v>-12792773</v>
       </c>
       <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="n">
+        <v>388322</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>-23279782</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -983,6 +1011,12 @@
       </c>
       <c r="AG5" t="inlineStr"/>
       <c r="AH5" t="inlineStr"/>
+      <c r="AI5" t="n">
+        <v>1013241</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>146092</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1069,6 +1103,12 @@
       <c r="AF6" t="inlineStr"/>
       <c r="AG6" t="inlineStr"/>
       <c r="AH6" t="inlineStr"/>
+      <c r="AI6" t="n">
+        <v>60257934</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>12862123</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1159,6 +1199,12 @@
         <v>213133</v>
       </c>
       <c r="AH7" t="inlineStr"/>
+      <c r="AI7" t="n">
+        <v>3837</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>11942</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1239,6 +1285,12 @@
       <c r="AF8" t="inlineStr"/>
       <c r="AG8" t="inlineStr"/>
       <c r="AH8" t="inlineStr"/>
+      <c r="AI8" t="n">
+        <v>4688209</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>18752997</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1331,6 +1383,12 @@
         <v>5600000000</v>
       </c>
       <c r="AH9" t="inlineStr"/>
+      <c r="AI9" t="n">
+        <v>1545113804</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>783324574</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1421,6 +1479,12 @@
         <v>130022</v>
       </c>
       <c r="AH10" t="inlineStr"/>
+      <c r="AI10" t="n">
+        <v>-63747719</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>-116044425</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -1509,6 +1573,12 @@
       </c>
       <c r="AG11" t="inlineStr"/>
       <c r="AH11" t="inlineStr"/>
+      <c r="AI11" t="n">
+        <v>7833024</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>5999293</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -1595,6 +1665,12 @@
       </c>
       <c r="AG12" t="inlineStr"/>
       <c r="AH12" t="inlineStr"/>
+      <c r="AI12" t="n">
+        <v>2800303</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>-514739</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -1657,6 +1733,8 @@
       <c r="AF13" t="inlineStr"/>
       <c r="AG13" t="inlineStr"/>
       <c r="AH13" t="inlineStr"/>
+      <c r="AI13" t="inlineStr"/>
+      <c r="AJ13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -1745,6 +1823,12 @@
       </c>
       <c r="AG14" t="inlineStr"/>
       <c r="AH14" t="inlineStr"/>
+      <c r="AI14" t="n">
+        <v>64890640</v>
+      </c>
+      <c r="AJ14" t="n">
+        <v>1745473</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -1825,6 +1909,12 @@
         <v>180682287</v>
       </c>
       <c r="AH15" t="inlineStr"/>
+      <c r="AI15" t="n">
+        <v>19794337</v>
+      </c>
+      <c r="AJ15" t="n">
+        <v>3506904</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -1915,6 +2005,12 @@
         <v>636025</v>
       </c>
       <c r="AH16" t="inlineStr"/>
+      <c r="AI16" t="n">
+        <v>35006</v>
+      </c>
+      <c r="AJ16" t="n">
+        <v>2986</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -1999,6 +2095,12 @@
       </c>
       <c r="AG17" t="inlineStr"/>
       <c r="AH17" t="inlineStr"/>
+      <c r="AI17" t="n">
+        <v>-1770749</v>
+      </c>
+      <c r="AJ17" t="n">
+        <v>104868</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -2097,6 +2199,12 @@
         <v>10145887709</v>
       </c>
       <c r="AH18" t="inlineStr"/>
+      <c r="AI18" t="n">
+        <v>9970455392</v>
+      </c>
+      <c r="AJ18" t="n">
+        <v>-1811884569</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -2141,6 +2249,8 @@
       <c r="AF19" t="inlineStr"/>
       <c r="AG19" t="inlineStr"/>
       <c r="AH19" t="inlineStr"/>
+      <c r="AI19" t="inlineStr"/>
+      <c r="AJ19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -2235,6 +2345,12 @@
         <v>5480848</v>
       </c>
       <c r="AH20" t="inlineStr"/>
+      <c r="AI20" t="n">
+        <v>387397</v>
+      </c>
+      <c r="AJ20" t="n">
+        <v>-171441</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>